<commit_message>
updated example data file to remove issue with invisible NaN rows
</commit_message>
<xml_diff>
--- a/mastml/tests/csv/example_data.xlsx
+++ b/mastml/tests/csv/example_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10908"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11108"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ryanjacobs/PycharmProjects/MAST-ML/tests/csv/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ryanjacobs/anaconda3_python37/envs/mastml_test_2021-01-15_v2/lib/python3.7/site-packages/mastml/tests/csv/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A50DC04-3F88-2D49-938F-3607C7EA5039}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F0635E2-F080-AE4E-9245-FF119545917A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5580" yWindow="3560" windowWidth="27640" windowHeight="16940" xr2:uid="{A7985CBF-1A19-C847-878E-79F1B52F6E99}"/>
+    <workbookView xWindow="5580" yWindow="3260" windowWidth="27640" windowHeight="16940" xr2:uid="{A7985CBF-1A19-C847-878E-79F1B52F6E99}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,10 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -634,10 +637,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{22AF4B6A-7D5F-3A40-A617-4E672040C89E}">
-  <dimension ref="A1:Y431"/>
+  <dimension ref="A1:Y409"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I22" sqref="I22"/>
+    <sheetView tabSelected="1" topLeftCell="A391" workbookViewId="0">
+      <selection activeCell="G404" sqref="G404"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -30757,7 +30760,7 @@
         <v>27</v>
       </c>
       <c r="C387" s="1" t="str">
-        <f t="shared" ref="C387:C431" si="6">CONCATENATE(A387,B387)</f>
+        <f t="shared" ref="C387:C409" si="6">CONCATENATE(A387,B387)</f>
         <v>WSc</v>
       </c>
       <c r="D387" s="1">
@@ -32542,94 +32545,6 @@
       <c r="Y409" s="1">
         <v>-3.6959459030000001</v>
       </c>
-    </row>
-    <row r="410" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="C410" s="1"/>
-      <c r="D410" s="1"/>
-    </row>
-    <row r="411" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="C411" s="1"/>
-      <c r="D411" s="1"/>
-    </row>
-    <row r="412" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="C412" s="1"/>
-      <c r="D412" s="1"/>
-    </row>
-    <row r="413" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="C413" s="1"/>
-      <c r="D413" s="1"/>
-    </row>
-    <row r="414" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="C414" s="1"/>
-      <c r="D414" s="1"/>
-    </row>
-    <row r="415" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="C415" s="1"/>
-      <c r="D415" s="1"/>
-    </row>
-    <row r="416" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="C416" s="1"/>
-      <c r="D416" s="1"/>
-    </row>
-    <row r="417" spans="3:4" x14ac:dyDescent="0.2">
-      <c r="C417" s="1"/>
-      <c r="D417" s="1"/>
-    </row>
-    <row r="418" spans="3:4" x14ac:dyDescent="0.2">
-      <c r="C418" s="1"/>
-      <c r="D418" s="1"/>
-    </row>
-    <row r="419" spans="3:4" x14ac:dyDescent="0.2">
-      <c r="C419" s="1"/>
-      <c r="D419" s="1"/>
-    </row>
-    <row r="420" spans="3:4" x14ac:dyDescent="0.2">
-      <c r="C420" s="1"/>
-      <c r="D420" s="1"/>
-    </row>
-    <row r="421" spans="3:4" x14ac:dyDescent="0.2">
-      <c r="C421" s="1"/>
-      <c r="D421" s="1"/>
-    </row>
-    <row r="422" spans="3:4" x14ac:dyDescent="0.2">
-      <c r="C422" s="1"/>
-      <c r="D422" s="1"/>
-    </row>
-    <row r="423" spans="3:4" x14ac:dyDescent="0.2">
-      <c r="C423" s="1"/>
-      <c r="D423" s="1"/>
-    </row>
-    <row r="424" spans="3:4" x14ac:dyDescent="0.2">
-      <c r="C424" s="1"/>
-      <c r="D424" s="1"/>
-    </row>
-    <row r="425" spans="3:4" x14ac:dyDescent="0.2">
-      <c r="C425" s="1"/>
-      <c r="D425" s="1"/>
-    </row>
-    <row r="426" spans="3:4" x14ac:dyDescent="0.2">
-      <c r="C426" s="1"/>
-      <c r="D426" s="1"/>
-    </row>
-    <row r="427" spans="3:4" x14ac:dyDescent="0.2">
-      <c r="C427" s="1"/>
-      <c r="D427" s="1"/>
-    </row>
-    <row r="428" spans="3:4" x14ac:dyDescent="0.2">
-      <c r="C428" s="1"/>
-      <c r="D428" s="1"/>
-    </row>
-    <row r="429" spans="3:4" x14ac:dyDescent="0.2">
-      <c r="C429" s="1"/>
-      <c r="D429" s="1"/>
-    </row>
-    <row r="430" spans="3:4" x14ac:dyDescent="0.2">
-      <c r="C430" s="1"/>
-      <c r="D430" s="1"/>
-    </row>
-    <row r="431" spans="3:4" x14ac:dyDescent="0.2">
-      <c r="C431" s="1"/>
-      <c r="D431" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>